<commit_message>
do func: import TPDL (NPOI)
</commit_message>
<xml_diff>
--- a/banhang24/Template/ImportExcel/FileImport_ThanhPhanDinhLuong.xlsx
+++ b/banhang24/Template/ImportExcel/FileImport_ThanhPhanDinhLuong.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10 TIMT\Source\repos\banhang24\banhang24\Template\ImportExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\KangjinDemo2\KangJinDemo\banhang24\Template\ImportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -154,17 +154,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -291,62 +282,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,281 +607,235 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="17" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="16" customWidth="1"/>
     <col min="5" max="5" width="55" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="14">
         <v>50000</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="7">
         <v>2</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="7">
         <v>7</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="14">
         <v>200000</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>4</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="8">
         <v>0.15</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="15" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="15" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="15">
         <v>300000</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="8">
         <v>2</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="15" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="8">
         <v>3</v>
       </c>
-      <c r="D12" s="27"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="15" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="8">
         <v>4</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="16" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="8">
         <v>5</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="8">
         <v>2.5</v>
       </c>
-      <c r="D15" s="27"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D16" s="27"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="15" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="8">
         <v>4</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="H4:K4"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>